<commit_message>
GPLIM-2980 backed out HSSFDataFormatter; continued work on persistence test
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ControlReagents.xlsx
+++ b/mercury/src/test/resources/testdata/ControlReagents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>tube barcode</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>NO_TEMPLATE_CONTROL</t>
+  </si>
+  <si>
+    <t>SK-2345</t>
   </si>
 </sst>
 </file>
@@ -395,9 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -456,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2">
         <v>42004</v>

</xml_diff>